<commit_message>
Updated code & data
</commit_message>
<xml_diff>
--- a/data/Low temp Hackathon 1135.xlsx
+++ b/data/Low temp Hackathon 1135.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/30040636/Dev/sub-zero/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7288597-E567-F945-8645-E4B35A21B1E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7A8CD5-8B55-5441-9400-6793CA0BABEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="17340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Humans" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="34">
   <si>
     <t>statement</t>
   </si>
@@ -470,11 +470,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M1000"/>
+  <dimension ref="A1:M996"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -728,7 +728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -1221,8 +1221,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="13" x14ac:dyDescent="0.15">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="A19" s="6"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -14913,64 +14912,8 @@
       <c r="L996" s="5"/>
       <c r="M996" s="5"/>
     </row>
-    <row r="997" spans="1:13" ht="13" x14ac:dyDescent="0.15">
-      <c r="A997" s="6"/>
-      <c r="C997" s="4"/>
-      <c r="D997" s="4"/>
-      <c r="E997" s="4"/>
-      <c r="F997" s="4"/>
-      <c r="G997" s="4"/>
-      <c r="H997" s="4"/>
-      <c r="I997" s="5"/>
-      <c r="J997" s="5"/>
-      <c r="K997" s="5"/>
-      <c r="L997" s="5"/>
-      <c r="M997" s="5"/>
-    </row>
-    <row r="998" spans="1:13" ht="13" x14ac:dyDescent="0.15">
-      <c r="A998" s="6"/>
-      <c r="C998" s="4"/>
-      <c r="D998" s="4"/>
-      <c r="E998" s="4"/>
-      <c r="F998" s="4"/>
-      <c r="G998" s="4"/>
-      <c r="H998" s="4"/>
-      <c r="I998" s="5"/>
-      <c r="J998" s="5"/>
-      <c r="K998" s="5"/>
-      <c r="L998" s="5"/>
-      <c r="M998" s="5"/>
-    </row>
-    <row r="999" spans="1:13" ht="13" x14ac:dyDescent="0.15">
-      <c r="A999" s="6"/>
-      <c r="C999" s="4"/>
-      <c r="D999" s="4"/>
-      <c r="E999" s="4"/>
-      <c r="F999" s="4"/>
-      <c r="G999" s="4"/>
-      <c r="H999" s="4"/>
-      <c r="I999" s="5"/>
-      <c r="J999" s="5"/>
-      <c r="K999" s="5"/>
-      <c r="L999" s="5"/>
-      <c r="M999" s="5"/>
-    </row>
-    <row r="1000" spans="1:13" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1000" s="6"/>
-      <c r="C1000" s="4"/>
-      <c r="D1000" s="4"/>
-      <c r="E1000" s="4"/>
-      <c r="F1000" s="4"/>
-      <c r="G1000" s="4"/>
-      <c r="H1000" s="4"/>
-      <c r="I1000" s="5"/>
-      <c r="J1000" s="5"/>
-      <c r="K1000" s="5"/>
-      <c r="L1000" s="5"/>
-      <c r="M1000" s="5"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A1000">
+  <conditionalFormatting sqref="A1:A996">
     <cfRule type="notContainsBlanks" dxfId="2" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
@@ -14984,10 +14927,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Y1000"/>
+  <dimension ref="A1:Y993"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:M36"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -14997,7 +14940,7 @@
     <col min="13" max="13" width="38.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -15058,7 +15001,7 @@
         <v>14</v>
       </c>
       <c r="C2" s="7">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="D2" s="7">
         <v>0.9</v>
@@ -15759,26 +15702,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
+    <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="1"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
+    <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="1"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1"/>
@@ -15861,25 +15804,25 @@
     <row r="52" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="1"/>
     </row>
-    <row r="54" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="1"/>
     </row>
-    <row r="55" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="1"/>
     </row>
-    <row r="56" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="1"/>
     </row>
-    <row r="59" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A59" s="1"/>
     </row>
     <row r="60" spans="1:1" ht="13" x14ac:dyDescent="0.15">
@@ -18684,29 +18627,8 @@
     <row r="993" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A993" s="1"/>
     </row>
-    <row r="994" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A994" s="1"/>
-    </row>
-    <row r="995" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A995" s="1"/>
-    </row>
-    <row r="996" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A996" s="1"/>
-    </row>
-    <row r="997" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A997" s="1"/>
-    </row>
-    <row r="998" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A998" s="1"/>
-    </row>
-    <row r="999" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A999" s="1"/>
-    </row>
-    <row r="1000" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1000" s="1"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A1000">
+  <conditionalFormatting sqref="A1:A993">
     <cfRule type="notContainsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
@@ -18722,13 +18644,13 @@
   </sheetPr>
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:M36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -18769,10 +18691,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="C2" s="1">
         <v>0.85</v>
       </c>
@@ -18807,10 +18732,13 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="C3" s="1">
         <v>0.7</v>
       </c>
@@ -18845,10 +18773,13 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C4" s="1">
         <v>0.2</v>
       </c>
@@ -18883,9 +18814,12 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C5" s="1">
         <v>0.8</v>
@@ -18925,6 +18859,9 @@
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C6" s="1">
         <v>0</v>
       </c>
@@ -18959,10 +18896,13 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C7" s="1">
         <v>0.2</v>
       </c>
@@ -18997,9 +18937,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C8" s="1">
         <v>0.2</v>
@@ -19039,6 +18982,9 @@
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C9" s="1">
         <v>0.2</v>
       </c>
@@ -19077,6 +19023,9 @@
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="C10" s="1">
         <v>0.85</v>
       </c>
@@ -19115,6 +19064,9 @@
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="C11" s="1">
         <v>0.85</v>
       </c>
@@ -19153,6 +19105,9 @@
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="B12" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="C12" s="1">
         <v>0.8</v>
       </c>
@@ -19191,6 +19146,9 @@
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="C13" s="1">
         <v>0.6</v>
       </c>
@@ -19229,6 +19187,9 @@
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="B14" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="C14" s="1">
         <v>0.8</v>
       </c>
@@ -19267,6 +19228,9 @@
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="B15" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C15" s="1">
         <v>0.2</v>
       </c>
@@ -19305,6 +19269,9 @@
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="B16" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="C16" s="1">
         <v>0.85</v>
       </c>
@@ -19343,6 +19310,9 @@
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="B17" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="C17" s="1">
         <v>0.85</v>
       </c>
@@ -19380,6 +19350,9 @@
     <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>32</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C18" s="1">
         <v>0.85</v>

</xml_diff>